<commit_message>
add info in studentprofile
</commit_message>
<xml_diff>
--- a/static/xlsxforms/School_Student_File.xlsx
+++ b/static/xlsxforms/School_Student_File.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -38,63 +38,6 @@
   </si>
   <si>
     <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unique_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">weight_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">height_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bmi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waist</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waist_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hip_circumference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hip_unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waist_to_height_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waist_to_height_ratio_derived</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nutri_leader</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school_coordinator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">school_contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uploaded_photo</t>
   </si>
 </sst>
 </file>
@@ -175,7 +118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -186,10 +129,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -209,39 +148,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA1" activeCellId="0" sqref="A:AA"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="4.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="5.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="7.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="25.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="12.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="13.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="7.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1010" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="990" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -263,63 +183,6 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" s="0" t="s">
-        <v>24</v>
-      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>